<commit_message>
:bento: every week analyize
</commit_message>
<xml_diff>
--- a/附件/每周效率统计.xlsx
+++ b/附件/每周效率统计.xlsx
@@ -37,9 +37,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -50,6 +50,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -57,15 +93,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -80,14 +149,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -95,44 +164,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,40 +187,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,31 +203,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,145 +377,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,6 +402,51 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -430,56 +475,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,10 +502,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -514,133 +514,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -970,13 +970,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9.375"/>
     <col min="4" max="4" width="16.625" customWidth="1"/>
@@ -1016,6 +1016,23 @@
         <v>0.72</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>43164</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.89</v>
+      </c>
+      <c r="D3">
+        <v>0.76</v>
+      </c>
+      <c r="E3">
+        <v>0.91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>

<commit_message>
update weekly mission analyize
</commit_message>
<xml_diff>
--- a/附件/每周效率统计.xlsx
+++ b/附件/每周效率统计.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9">
   <si>
     <t>起始日期</t>
   </si>
@@ -30,16 +30,28 @@
   <si>
     <t>总完成率</t>
   </si>
+  <si>
+    <t>cont数</t>
+  </si>
+  <si>
+    <t>new数</t>
+  </si>
+  <si>
+    <t>(2/2)</t>
+  </si>
+  <si>
+    <t>23/25</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -50,6 +62,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -58,8 +112,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -72,69 +127,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,13 +166,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -163,32 +174,33 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,91 +221,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,85 +389,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,15 +406,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -417,6 +420,48 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -453,39 +498,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -502,10 +514,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -514,141 +526,144 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -970,19 +985,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="9.375"/>
+    <col min="1" max="1" width="10.375"/>
     <col min="4" max="4" width="16.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -997,6 +1012,12 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1031,6 +1052,29 @@
       </c>
       <c r="E3">
         <v>0.91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>43171</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.91</v>
+      </c>
+      <c r="D4">
+        <v>0.84</v>
+      </c>
+      <c r="E4">
+        <v>0.92</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>